<commit_message>
new tlp profiles and some new scripts
</commit_message>
<xml_diff>
--- a/lichtblick/tlp/sourcedata/Avacon_HZ0.xlsx
+++ b/lichtblick/tlp/sourcedata/Avacon_HZ0.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://lichtblickit-my.sharepoint.com/personal/ruud_wijtvliet_lichtblick_de/Documents/Work_in_RM/python/2019_07_lichtblick/lichtblick/tlp/sourcedata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{71E102A1-688A-409A-B87F-400F3697DA38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{71E102A1-688A-409A-B87F-400F3697DA38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9A351F77-C692-4258-A743-D02AD209FFE1}"/>
   <bookViews>
     <workbookView xWindow="1620" yWindow="-110" windowWidth="36890" windowHeight="21820" xr2:uid="{5FD08CA9-8031-4678-B173-E34E23EE75F0}"/>
   </bookViews>
   <sheets>
     <sheet name="HZ0" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" calcOnSave="0"/>
+  <calcPr calcId="191029" refMode="R1C1" calcOnSave="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -43,7 +43,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -76,7 +76,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -394,7 +394,7 @@
   <dimension ref="A1:AK97"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11372,6 +11372,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100E7B6664B53D93F468A814C7991F8EAFE" ma:contentTypeVersion="7" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="ff3dc54043d9b88bfb9aa7ef8f6bf51c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b4e78a58-83f1-44b2-98d1-81c9abb66313" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5c35705ade9ad5c05bdfe9d6496ac8c3" ns3:_="">
     <xsd:import namespace="b4e78a58-83f1-44b2-98d1-81c9abb66313"/>
@@ -11535,15 +11544,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -11551,6 +11551,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87AEF669-F188-42C6-A972-976F01D15DEA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FECAEED6-95CC-4036-B3B2-466D16AF91BB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11568,14 +11576,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87AEF669-F188-42C6-A972-976F01D15DEA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C314730D-77BB-4144-9B22-D99746A841C4}">
   <ds:schemaRefs>

</xml_diff>